<commit_message>
Product price retrieval to excel
</commit_message>
<xml_diff>
--- a/Test/src/testData/TestData.xlsx
+++ b/Test/src/testData/TestData.xlsx
@@ -16,27 +16,141 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="45">
+  <si>
+    <t>Sony 80 cm (32 inches) Bravia KLV-32R302E HD Ready LED TV</t>
+  </si>
+  <si>
+    <t>₹23,490.₹23,490</t>
+  </si>
+  <si>
+    <t>Sony 59.9 cm (24 inches) Bravia KLV-24P413D HD Ready LED TV (Black)</t>
+  </si>
+  <si>
+    <t>₹14,490.₹14,490</t>
+  </si>
   <si>
     <t>Sony 80 cm (32 inches) Bravia KLV-32W512D HD Ready Smart LED TV</t>
   </si>
   <si>
+    <t>₹27,990.₹27,990</t>
+  </si>
+  <si>
+    <t>Sony 80.1 cm (32 inches) Bravia KLV-32W672E Full HD LED Smart TV (Black)</t>
+  </si>
+  <si>
+    <t>₹34,990.₹34,990</t>
+  </si>
+  <si>
+    <t>Sony 108 cm (43 inches) Bravia KD-43X7500E 4K UHD LED Smart TV (Black)</t>
+  </si>
+  <si>
+    <t>₹64,500.₹64,500</t>
+  </si>
+  <si>
+    <t>Sony 101.4 cm (40 inches) KLV-40W672E Full HD LED Smart TV</t>
+  </si>
+  <si>
+    <t>₹47,489.₹47,489</t>
+  </si>
+  <si>
+    <t>Sony 101.6 cm (40 inches) Bravia KLV-40W562D Full HD LED Smart TV (Black)</t>
+  </si>
+  <si>
+    <t>₹45,990.₹45,990</t>
+  </si>
+  <si>
+    <t>Sony 108 cm (43 inches) Bravia KD-43X7002E 4K UHD LED Smart TV</t>
+  </si>
+  <si>
+    <t>₹60,500.₹60,500</t>
+  </si>
+  <si>
+    <t>Sony 72.4 cm (29 inches) BRAVIA KLV-29P423D HD Ready LED TV</t>
+  </si>
+  <si>
+    <t>₹19,990.₹19,990</t>
+  </si>
+  <si>
+    <t>Sony 80 cm (32 inches) Bravia KLV-32R412D HD Ready LED TV</t>
+  </si>
+  <si>
+    <t>₹25,990.₹25,990</t>
+  </si>
+  <si>
+    <t>Sony 108cm (43 inches) KLV-43W772E Full HD LED Smart TV</t>
+  </si>
+  <si>
+    <t>₹52,350.₹52,350</t>
+  </si>
+  <si>
+    <t>Sony 101.6 cm (40 inches) Bravia KLV-40W562D Full HD Smart LED TV</t>
+  </si>
+  <si>
+    <t>₹49,999.₹49,999</t>
+  </si>
+  <si>
+    <t>Sony 123.2 cm (49 inches) Bravia KLV-49W672E Full HD Smart LED TV</t>
+  </si>
+  <si>
+    <t>₹61,400.₹61,400</t>
+  </si>
+  <si>
+    <t>Sony 138.8 cm (55 inches) Bravia KD-55X7002E 4K UHD LED Smart TV</t>
+  </si>
+  <si>
+    <t>₹98,400.₹98,400</t>
+  </si>
+  <si>
+    <t>Sony 80.0 cm (32 inches) KLV-W512D HD Ready LED Smart TV (Black)</t>
+  </si>
+  <si>
+    <t>  29,500</t>
+  </si>
+  <si>
+    <t>Sony 108 cm (43 inches) Bravia KDL-43W800D Full HD 3D LED Android TV</t>
+  </si>
+  <si>
+    <t>₹63,900.₹63,900</t>
+  </si>
+  <si>
+    <t>Sony 123.2 cm (49 inches) BRAVIA KLV-49W772E Full HD Smart LED TV</t>
+  </si>
+  <si>
+    <t>₹69,200.₹69,200</t>
+  </si>
+  <si>
+    <t>Sony 101.6 cm (40 inches) Bravia KLV-40R352E Full HD LED TV</t>
+  </si>
+  <si>
+    <t>₹41,990.₹41,990</t>
+  </si>
+  <si>
+    <t>Sony 138.8 cm (55 inches) Bravia KD-55X8200E 4K UHD LED Smart TV</t>
+  </si>
+  <si>
+    <t>₹1,12,970.₹1,12,970</t>
+  </si>
+  <si>
+    <t>Sony 80 cm (32 inches) Bravia KLV-32W622E HD Ready LED Smart TV (Black)</t>
+  </si>
+  <si>
+    <t>₹30,990.₹30,990</t>
+  </si>
+  <si>
+    <t>₹59,389.₹59,389</t>
+  </si>
+  <si>
+    <t>₹52,000.₹52,000</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Sony 59.9 cm (24 inches) Bravia KLV-24P413D HD Ready LED TV (Black)</t>
-  </si>
-  <si>
-    <t>Sony 80 cm (32 inches) Bravia KLV-32R302E HD Ready LED TV</t>
-  </si>
-  <si>
-    <t>Sony 80.1 cm (32 inches) Bravia KLV-32W672E Full HD LED Smart TV (Black)</t>
-  </si>
-  <si>
-    <t>Sony 108cm (43 inches) KLV-43W772E Full HD LED Smart TV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  </t>
+    <t>  29,500.00</t>
+  </si>
+  <si>
+    <t>₹69,000.₹69,000</t>
   </si>
 </sst>
 </file>
@@ -369,9 +483,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -386,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -394,31 +510,151 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>